<commit_message>
added Register and updated home step, page,tree
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/ExcelData.xlsx
+++ b/target/test-classes/TestData/ExcelData.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{FB0F5173-F269-4C9C-8981-73D262CF8FF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="code" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="E1:T27"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>username</t>
   </si>
@@ -61,9 +59,6 @@
     <t>Ilike swEEt5</t>
   </si>
   <si>
-    <t>rabi%di3</t>
-  </si>
-  <si>
     <t>Panipuri</t>
   </si>
   <si>
@@ -218,12 +213,48 @@
   </si>
   <si>
     <t>Logged out successfully</t>
+  </si>
+  <si>
+    <t>edgr7&amp;rk</t>
+  </si>
+  <si>
+    <t>invalid$$$$</t>
+  </si>
+  <si>
+    <t>NewUser</t>
+  </si>
+  <si>
+    <t>SyntaxError: bad input on line 1</t>
+  </si>
+  <si>
+    <t>ActionSquad#%^&amp;</t>
+  </si>
+  <si>
+    <t>NameError: name 'edgr7' is not defined on line 1</t>
+  </si>
+  <si>
+    <t>Invalid Password</t>
+  </si>
+  <si>
+    <t>password_mismatch:The two password fields didn’t match.</t>
+  </si>
+  <si>
+    <t>The user Is already Registered</t>
+  </si>
+  <si>
+    <t>New Account Created.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Invalid Username </t>
+  </si>
+  <si>
+    <t>Login</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -267,7 +298,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -290,12 +321,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -305,6 +347,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -401,23 +446,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -453,23 +481,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -645,25 +656,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.5546875" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" customWidth="1"/>
+    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -677,16 +689,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
-        <v>61</v>
-      </c>
       <c r="G1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -700,16 +712,16 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F2" t="s">
         <v>62</v>
       </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
       <c r="G2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -722,256 +734,292 @@
       <c r="D3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D6" s="2" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="3" t="s">
+    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D8" s="3" t="s">
+    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="2" t="s">
+    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="3" t="s">
+    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="3" t="s">
+    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="3" t="s">
+    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="3" t="s">
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="2" t="s">
+    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="3" t="s">
+    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="3" t="s">
+    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="3" t="s">
+    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="3" t="s">
+    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="3" t="s">
+    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="3" t="s">
+    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="2" t="s">
+    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="2" t="s">
+    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="4" t="s">
+    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D24" s="4" t="s">
+    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="3" t="s">
+    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="2" t="s">
+    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="4:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="3" t="s">
+    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D29" s="3" t="s">
+    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="30" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="3" t="s">
+    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="3" t="s">
+    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="3" t="s">
+    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="3" t="s">
+    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="3" t="s">
+    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D35" s="2" t="s">
+    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D37" s="2" t="s">
+    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="3" t="s">
+    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="3" t="s">
+    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="40" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D40" s="3" t="s">
+    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D41" s="3" t="s">
+    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="3" t="s">
+    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="2" t="s">
+    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D44" s="3" t="s">
+    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D45" s="3" t="s">
-        <v>59</v>
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D46" s="5" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test runner class
</commit_message>
<xml_diff>
--- a/target/test-classes/TestData/ExcelData.xlsx
+++ b/target/test-classes/TestData/ExcelData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24332"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7894D5A0-C75A-4D75-ACD2-594E63BA9D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="13890"/>
+    <workbookView xWindow="2232" yWindow="2232" windowWidth="17280" windowHeight="9960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -104,9 +105,6 @@
     <t>Introduction</t>
   </si>
   <si>
-    <t>Creating Linked LIst</t>
-  </si>
-  <si>
     <t>Types of Linked List</t>
   </si>
   <si>
@@ -249,12 +247,15 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t>Creating Linked List</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -446,6 +447,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -481,6 +499,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -656,26 +691,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5546875" customWidth="1"/>
+    <col min="2" max="2" width="54.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,16 +724,16 @@
         <v>10</v>
       </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
         <v>59</v>
       </c>
-      <c r="F1" t="s">
-        <v>60</v>
-      </c>
       <c r="G1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -712,16 +747,16 @@
         <v>12</v>
       </c>
       <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
         <v>61</v>
       </c>
-      <c r="F2" t="s">
-        <v>62</v>
-      </c>
       <c r="G2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -735,21 +770,21 @@
         <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -763,248 +798,248 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
-      </c>
-      <c r="B8" t="s">
-        <v>71</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D17" s="3" t="s">
+    <row r="18" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="3" t="s">
+    <row r="19" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="3" t="s">
+    <row r="20" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="3" t="s">
+    <row r="21" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="2" t="s">
+    <row r="22" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="2" t="s">
+    <row r="23" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="4" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="4" t="s">
+    <row r="24" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="4" t="s">
+    <row r="25" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="25" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D25" s="3" t="s">
+    <row r="26" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="2" t="s">
+    <row r="27" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D27" s="3" t="s">
+    <row r="28" spans="4:4" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="4:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D28" s="3" t="s">
+    <row r="29" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="29" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D29" s="3" t="s">
+    <row r="30" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="30" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D30" s="3" t="s">
+    <row r="31" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D31" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D31" s="3" t="s">
+    <row r="32" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D32" s="3" t="s">
+    <row r="33" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D33" s="3" t="s">
+    <row r="34" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D34" s="3" t="s">
+    <row r="35" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="2" t="s">
+    <row r="36" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="2" t="s">
+    <row r="37" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="2" t="s">
+    <row r="38" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D38" s="3" t="s">
+    <row r="39" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="39" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D39" s="3" t="s">
+    <row r="40" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="40" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D40" s="3" t="s">
+    <row r="41" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="41" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D41" s="3" t="s">
+    <row r="42" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D42" s="3" t="s">
+    <row r="43" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="43" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D43" s="2" t="s">
+    <row r="44" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D44" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="44" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D44" s="3" t="s">
+    <row r="45" spans="4:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="45" spans="4:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D45" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D46" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A8" r:id="rId2" display="ActionSquad@#%^&amp;" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -1012,14 +1047,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>